<commit_message>
Add basic models for AMOP
</commit_message>
<xml_diff>
--- a/Data/AMAN/AaCOE_CapenPark_Daily-Weather_20180601-20190531.xlsx
+++ b/Data/AMAN/AaCOE_CapenPark_Daily-Weather_20180601-20190531.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Dropbox\SERDP_Phenology\Pens\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\messe\Documents\GitHub\JuvenileEmigrationPhenology\Data\AMAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D4823F-CD28-4DBE-A328-824148384C12}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2734652-0BB1-46E3-84F5-2AA15B6816C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D5D19BDA-A0D1-48CB-812F-444A33C3CB0D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D5D19BDA-A0D1-48CB-812F-444A33C3CB0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +24,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1525,27 +1529,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8FF5C27-94FC-4CA2-AE0B-156014607FE1}">
   <dimension ref="A1:O366"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="K55" workbookViewId="0">
+      <selection activeCell="M67" sqref="M67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="20.81640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1592,7 +1596,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>304</v>
       </c>
@@ -1639,7 +1643,7 @@
         <v>26.17</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>305</v>
       </c>
@@ -1686,7 +1690,7 @@
         <v>13.71</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>306</v>
       </c>
@@ -1733,7 +1737,7 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>307</v>
       </c>
@@ -1780,7 +1784,7 @@
         <v>15.27</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>308</v>
       </c>
@@ -1827,7 +1831,7 @@
         <v>25.99</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>309</v>
       </c>
@@ -1874,7 +1878,7 @@
         <v>23.3</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>310</v>
       </c>
@@ -1921,7 +1925,7 @@
         <v>19.03</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>311</v>
       </c>
@@ -1968,7 +1972,7 @@
         <v>18.809999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>312</v>
       </c>
@@ -2015,7 +2019,7 @@
         <v>22.64</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>313</v>
       </c>
@@ -2062,7 +2066,7 @@
         <v>23.16</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>314</v>
       </c>
@@ -2109,7 +2113,7 @@
         <v>24.18</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>315</v>
       </c>
@@ -2156,7 +2160,7 @@
         <v>20.95</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>316</v>
       </c>
@@ -2203,7 +2207,7 @@
         <v>22.09</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>317</v>
       </c>
@@ -2250,7 +2254,7 @@
         <v>20.94</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>318</v>
       </c>
@@ -2297,7 +2301,7 @@
         <v>24.78</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>319</v>
       </c>
@@ -2344,7 +2348,7 @@
         <v>24.13</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>320</v>
       </c>
@@ -2391,7 +2395,7 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>321</v>
       </c>
@@ -2438,7 +2442,7 @@
         <v>22.94</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>322</v>
       </c>
@@ -2485,7 +2489,7 @@
         <v>17.420000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>323</v>
       </c>
@@ -2532,7 +2536,7 @@
         <v>19.059999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>324</v>
       </c>
@@ -2579,7 +2583,7 @@
         <v>12.26</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>325</v>
       </c>
@@ -2626,7 +2630,7 @@
         <v>7.02</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>326</v>
       </c>
@@ -2673,7 +2677,7 @@
         <v>17.940000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>327</v>
       </c>
@@ -2720,7 +2724,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>328</v>
       </c>
@@ -2767,7 +2771,7 @@
         <v>20.11</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>329</v>
       </c>
@@ -2814,7 +2818,7 @@
         <v>1.59</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>330</v>
       </c>
@@ -2861,7 +2865,7 @@
         <v>20.22</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>331</v>
       </c>
@@ -2908,7 +2912,7 @@
         <v>23.01</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>332</v>
       </c>
@@ -2955,7 +2959,7 @@
         <v>25.28</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>333</v>
       </c>
@@ -3002,7 +3006,7 @@
         <v>24.43</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>334</v>
       </c>
@@ -3049,7 +3053,7 @@
         <v>18.02</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>335</v>
       </c>
@@ -3096,7 +3100,7 @@
         <v>23.3</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>336</v>
       </c>
@@ -3143,7 +3147,7 @@
         <v>19.95</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>337</v>
       </c>
@@ -3190,7 +3194,7 @@
         <v>23.46</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>338</v>
       </c>
@@ -3237,7 +3241,7 @@
         <v>24.65</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>339</v>
       </c>
@@ -3284,7 +3288,7 @@
         <v>22.54</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>340</v>
       </c>
@@ -3331,7 +3335,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>341</v>
       </c>
@@ -3378,7 +3382,7 @@
         <v>25.27</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>342</v>
       </c>
@@ -3425,7 +3429,7 @@
         <v>20.89</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>343</v>
       </c>
@@ -3472,7 +3476,7 @@
         <v>22.96</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>344</v>
       </c>
@@ -3519,7 +3523,7 @@
         <v>22.71</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>345</v>
       </c>
@@ -3566,7 +3570,7 @@
         <v>24.09</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>346</v>
       </c>
@@ -3613,7 +3617,7 @@
         <v>22.93</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>347</v>
       </c>
@@ -3660,7 +3664,7 @@
         <v>18.27</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>348</v>
       </c>
@@ -3707,7 +3711,7 @@
         <v>21.04</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>349</v>
       </c>
@@ -3754,7 +3758,7 @@
         <v>21.73</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>350</v>
       </c>
@@ -3801,7 +3805,7 @@
         <v>15.16</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>351</v>
       </c>
@@ -3848,7 +3852,7 @@
         <v>12.95</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>352</v>
       </c>
@@ -3895,7 +3899,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>353</v>
       </c>
@@ -3942,7 +3946,7 @@
         <v>21.94</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>354</v>
       </c>
@@ -3989,7 +3993,7 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>355</v>
       </c>
@@ -4036,7 +4040,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>356</v>
       </c>
@@ -4083,7 +4087,7 @@
         <v>19.170000000000002</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>357</v>
       </c>
@@ -4130,7 +4134,7 @@
         <v>20.350000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>358</v>
       </c>
@@ -4177,7 +4181,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>359</v>
       </c>
@@ -4224,7 +4228,7 @@
         <v>8.2200000000000006</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>360</v>
       </c>
@@ -4271,7 +4275,7 @@
         <v>24.1</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>361</v>
       </c>
@@ -4318,7 +4322,7 @@
         <v>15.05</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>362</v>
       </c>
@@ -4365,7 +4369,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>363</v>
       </c>
@@ -4412,7 +4416,7 @@
         <v>14.24</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>364</v>
       </c>
@@ -4459,7 +4463,7 @@
         <v>17.63</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>365</v>
       </c>
@@ -4506,7 +4510,7 @@
         <v>22.17</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>366</v>
       </c>
@@ -4553,7 +4557,7 @@
         <v>22.56</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>367</v>
       </c>
@@ -4600,7 +4604,7 @@
         <v>22.58</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>368</v>
       </c>
@@ -4647,7 +4651,7 @@
         <v>21.63</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>369</v>
       </c>
@@ -4694,7 +4698,7 @@
         <v>19.12</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>370</v>
       </c>
@@ -4741,7 +4745,7 @@
         <v>15.42</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>371</v>
       </c>
@@ -4788,7 +4792,7 @@
         <v>11.85</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>372</v>
       </c>
@@ -4835,7 +4839,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>373</v>
       </c>
@@ -4882,7 +4886,7 @@
         <v>20.07</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>374</v>
       </c>
@@ -4929,7 +4933,7 @@
         <v>17.93</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>375</v>
       </c>
@@ -4976,7 +4980,7 @@
         <v>20.87</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>376</v>
       </c>
@@ -5023,7 +5027,7 @@
         <v>20.75</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>377</v>
       </c>
@@ -5070,7 +5074,7 @@
         <v>18.059999999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>378</v>
       </c>
@@ -5117,7 +5121,7 @@
         <v>7.94</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>379</v>
       </c>
@@ -5164,7 +5168,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>15</v>
       </c>
@@ -5211,7 +5215,7 @@
         <v>19.55</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>16</v>
       </c>
@@ -5258,7 +5262,7 @@
         <v>16.66</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>17</v>
       </c>
@@ -5305,7 +5309,7 @@
         <v>14.42</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>18</v>
       </c>
@@ -5352,7 +5356,7 @@
         <v>12.12</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>19</v>
       </c>
@@ -5399,7 +5403,7 @@
         <v>10.75</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>20</v>
       </c>
@@ -5446,7 +5450,7 @@
         <v>16.09</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>21</v>
       </c>
@@ -5493,7 +5497,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>22</v>
       </c>
@@ -5540,7 +5544,7 @@
         <v>8.43</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>23</v>
       </c>
@@ -5587,7 +5591,7 @@
         <v>14.55</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>24</v>
       </c>
@@ -5634,7 +5638,7 @@
         <v>19.23</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>25</v>
       </c>
@@ -5681,7 +5685,7 @@
         <v>17.8</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>26</v>
       </c>
@@ -5728,7 +5732,7 @@
         <v>18.91</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>27</v>
       </c>
@@ -5775,7 +5779,7 @@
         <v>18.71</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>28</v>
       </c>
@@ -5822,7 +5826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>29</v>
       </c>
@@ -5869,7 +5873,7 @@
         <v>5.18</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>30</v>
       </c>
@@ -5916,7 +5920,7 @@
         <v>3.47</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>31</v>
       </c>
@@ -5963,7 +5967,7 @@
         <v>16.809999999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>32</v>
       </c>
@@ -6010,7 +6014,7 @@
         <v>14.64</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>33</v>
       </c>
@@ -6057,7 +6061,7 @@
         <v>15.46</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>34</v>
       </c>
@@ -6104,7 +6108,7 @@
         <v>15.33</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>35</v>
       </c>
@@ -6151,7 +6155,7 @@
         <v>12.73</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>36</v>
       </c>
@@ -6198,7 +6202,7 @@
         <v>6.35</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>37</v>
       </c>
@@ -6245,7 +6249,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>38</v>
       </c>
@@ -6292,7 +6296,7 @@
         <v>3.62</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>39</v>
       </c>
@@ -6339,7 +6343,7 @@
         <v>12.11</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>40</v>
       </c>
@@ -6386,7 +6390,7 @@
         <v>17.920000000000002</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>41</v>
       </c>
@@ -6433,7 +6437,7 @@
         <v>16.55</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>42</v>
       </c>
@@ -6480,7 +6484,7 @@
         <v>14.78</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>43</v>
       </c>
@@ -6527,7 +6531,7 @@
         <v>16.68</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>44</v>
       </c>
@@ -6574,7 +6578,7 @@
         <v>14.52</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>45</v>
       </c>
@@ -6621,7 +6625,7 @@
         <v>14.83</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>46</v>
       </c>
@@ -6668,7 +6672,7 @@
         <v>16.38</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>47</v>
       </c>
@@ -6715,7 +6719,7 @@
         <v>14.7</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>48</v>
       </c>
@@ -6762,7 +6766,7 @@
         <v>14.68</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>49</v>
       </c>
@@ -6809,7 +6813,7 @@
         <v>13.18</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>50</v>
       </c>
@@ -6856,7 +6860,7 @@
         <v>14.02</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
         <v>51</v>
       </c>
@@ -6903,7 +6907,7 @@
         <v>12.86</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
         <v>52</v>
       </c>
@@ -6950,7 +6954,7 @@
         <v>16.27</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
         <v>53</v>
       </c>
@@ -6997,7 +7001,7 @@
         <v>16.45</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>54</v>
       </c>
@@ -7044,7 +7048,7 @@
         <v>5.01</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>55</v>
       </c>
@@ -7091,7 +7095,7 @@
         <v>12.51</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
         <v>56</v>
       </c>
@@ -7138,7 +7142,7 @@
         <v>11.22</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
         <v>57</v>
       </c>
@@ -7185,7 +7189,7 @@
         <v>16.010000000000002</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
         <v>58</v>
       </c>
@@ -7232,7 +7236,7 @@
         <v>12.88</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
         <v>59</v>
       </c>
@@ -7279,7 +7283,7 @@
         <v>11.56</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
         <v>60</v>
       </c>
@@ -7326,7 +7330,7 @@
         <v>7.81</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
         <v>61</v>
       </c>
@@ -7373,7 +7377,7 @@
         <v>10.85</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
         <v>62</v>
       </c>
@@ -7420,7 +7424,7 @@
         <v>11.37</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
         <v>63</v>
       </c>
@@ -7467,7 +7471,7 @@
         <v>11.78</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
         <v>64</v>
       </c>
@@ -7514,7 +7518,7 @@
         <v>3.81</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
         <v>65</v>
       </c>
@@ -7561,7 +7565,7 @@
         <v>11.05</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
         <v>66</v>
       </c>
@@ -7608,7 +7612,7 @@
         <v>7.63</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>67</v>
       </c>
@@ -7655,7 +7659,7 @@
         <v>4.21</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
         <v>68</v>
       </c>
@@ -7702,7 +7706,7 @@
         <v>11.56</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>69</v>
       </c>
@@ -7749,7 +7753,7 @@
         <v>8.7899999999999991</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
         <v>70</v>
       </c>
@@ -7796,7 +7800,7 @@
         <v>6.11</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
         <v>71</v>
       </c>
@@ -7843,7 +7847,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
         <v>72</v>
       </c>
@@ -7890,7 +7894,7 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
         <v>73</v>
       </c>
@@ -7937,7 +7941,7 @@
         <v>5.86</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
         <v>74</v>
       </c>
@@ -7984,7 +7988,7 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
         <v>75</v>
       </c>
@@ -8031,7 +8035,7 @@
         <v>12.03</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
         <v>76</v>
       </c>
@@ -8078,7 +8082,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
         <v>77</v>
       </c>
@@ -8125,7 +8129,7 @@
         <v>13.33</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
         <v>78</v>
       </c>
@@ -8172,7 +8176,7 @@
         <v>13.05</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
         <v>79</v>
       </c>
@@ -8219,7 +8223,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>80</v>
       </c>
@@ -8266,7 +8270,7 @@
         <v>13.24</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
         <v>81</v>
       </c>
@@ -8313,7 +8317,7 @@
         <v>13.21</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
         <v>82</v>
       </c>
@@ -8360,7 +8364,7 @@
         <v>12.63</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
         <v>83</v>
       </c>
@@ -8407,7 +8411,7 @@
         <v>12.84</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
         <v>84</v>
       </c>
@@ -8454,7 +8458,7 @@
         <v>11.54</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
         <v>85</v>
       </c>
@@ -8501,7 +8505,7 @@
         <v>5.36</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
         <v>86</v>
       </c>
@@ -8548,7 +8552,7 @@
         <v>2.27</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
         <v>87</v>
       </c>
@@ -8595,7 +8599,7 @@
         <v>11.81</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
         <v>88</v>
       </c>
@@ -8642,7 +8646,7 @@
         <v>12.19</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
         <v>89</v>
       </c>
@@ -8689,7 +8693,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
         <v>90</v>
       </c>
@@ -8736,7 +8740,7 @@
         <v>5.83</v>
       </c>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>91</v>
       </c>
@@ -8783,7 +8787,7 @@
         <v>7.57</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
         <v>92</v>
       </c>
@@ -8830,7 +8834,7 @@
         <v>3.12</v>
       </c>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
         <v>93</v>
       </c>
@@ -8877,7 +8881,7 @@
         <v>4.45</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
         <v>94</v>
       </c>
@@ -8924,7 +8928,7 @@
         <v>5.55</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
         <v>95</v>
       </c>
@@ -8971,7 +8975,7 @@
         <v>1.44</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
         <v>96</v>
       </c>
@@ -9018,7 +9022,7 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
         <v>97</v>
       </c>
@@ -9065,7 +9069,7 @@
         <v>8.83</v>
       </c>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
         <v>98</v>
       </c>
@@ -9112,7 +9116,7 @@
         <v>10.69</v>
       </c>
     </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
         <v>99</v>
       </c>
@@ -9159,7 +9163,7 @@
         <v>4.7300000000000004</v>
       </c>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
         <v>100</v>
       </c>
@@ -9206,7 +9210,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
         <v>101</v>
       </c>
@@ -9253,7 +9257,7 @@
         <v>10.69</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
         <v>102</v>
       </c>
@@ -9300,7 +9304,7 @@
         <v>5.71</v>
       </c>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
         <v>103</v>
       </c>
@@ -9347,7 +9351,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
         <v>104</v>
       </c>
@@ -9394,7 +9398,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
         <v>105</v>
       </c>
@@ -9441,7 +9445,7 @@
         <v>10.19</v>
       </c>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
         <v>106</v>
       </c>
@@ -9488,7 +9492,7 @@
         <v>9.9600000000000009</v>
       </c>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
         <v>107</v>
       </c>
@@ -9535,7 +9539,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
         <v>108</v>
       </c>
@@ -9582,7 +9586,7 @@
         <v>5.65</v>
       </c>
     </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
         <v>109</v>
       </c>
@@ -9629,7 +9633,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
         <v>110</v>
       </c>
@@ -9676,7 +9680,7 @@
         <v>6.16</v>
       </c>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
         <v>111</v>
       </c>
@@ -9723,7 +9727,7 @@
         <v>8.49</v>
       </c>
     </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
         <v>112</v>
       </c>
@@ -9770,7 +9774,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
         <v>113</v>
       </c>
@@ -9817,7 +9821,7 @@
         <v>9.23</v>
       </c>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
         <v>114</v>
       </c>
@@ -9864,7 +9868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
         <v>115</v>
       </c>
@@ -9911,7 +9915,7 @@
         <v>8.01</v>
       </c>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A179" s="1" t="s">
         <v>116</v>
       </c>
@@ -9958,7 +9962,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
         <v>117</v>
       </c>
@@ -10005,7 +10009,7 @@
         <v>4.54</v>
       </c>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A181" s="1" t="s">
         <v>118</v>
       </c>
@@ -10052,7 +10056,7 @@
         <v>8.5500000000000007</v>
       </c>
     </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A182" s="1" t="s">
         <v>119</v>
       </c>
@@ -10099,7 +10103,7 @@
         <v>4.0199999999999996</v>
       </c>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="s">
         <v>120</v>
       </c>
@@ -10146,7 +10150,7 @@
         <v>5.93</v>
       </c>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A184" s="1" t="s">
         <v>121</v>
       </c>
@@ -10193,7 +10197,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
         <v>122</v>
       </c>
@@ -10240,7 +10244,7 @@
         <v>4.33</v>
       </c>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
         <v>123</v>
       </c>
@@ -10287,7 +10291,7 @@
         <v>1.94</v>
       </c>
     </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A187" s="1" t="s">
         <v>124</v>
       </c>
@@ -10334,7 +10338,7 @@
         <v>1.69</v>
       </c>
     </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A188" s="1" t="s">
         <v>125</v>
       </c>
@@ -10381,7 +10385,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A189" s="1" t="s">
         <v>126</v>
       </c>
@@ -10428,7 +10432,7 @@
         <v>8.32</v>
       </c>
     </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A190" s="1" t="s">
         <v>127</v>
       </c>
@@ -10475,7 +10479,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A191" s="1" t="s">
         <v>128</v>
       </c>
@@ -10522,7 +10526,7 @@
         <v>6.59</v>
       </c>
     </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A192" s="1" t="s">
         <v>129</v>
       </c>
@@ -10569,7 +10573,7 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A193" s="1" t="s">
         <v>130</v>
       </c>
@@ -10616,7 +10620,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A194" s="1" t="s">
         <v>131</v>
       </c>
@@ -10663,7 +10667,7 @@
         <v>8.02</v>
       </c>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A195" s="1" t="s">
         <v>132</v>
       </c>
@@ -10710,7 +10714,7 @@
         <v>7.41</v>
       </c>
     </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A196" s="1" t="s">
         <v>133</v>
       </c>
@@ -10757,7 +10761,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A197" s="1" t="s">
         <v>134</v>
       </c>
@@ -10804,7 +10808,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A198" s="1" t="s">
         <v>135</v>
       </c>
@@ -10851,7 +10855,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A199" s="1" t="s">
         <v>136</v>
       </c>
@@ -10898,7 +10902,7 @@
         <v>8.24</v>
       </c>
     </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
         <v>137</v>
       </c>
@@ -10945,7 +10949,7 @@
         <v>8.15</v>
       </c>
     </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A201" s="1" t="s">
         <v>138</v>
       </c>
@@ -10992,7 +10996,7 @@
         <v>8.06</v>
       </c>
     </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="s">
         <v>139</v>
       </c>
@@ -11039,7 +11043,7 @@
         <v>7.85</v>
       </c>
     </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A203" s="1" t="s">
         <v>140</v>
       </c>
@@ -11086,7 +11090,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A204" s="1" t="s">
         <v>141</v>
       </c>
@@ -11133,7 +11137,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A205" s="1" t="s">
         <v>142</v>
       </c>
@@ -11180,7 +11184,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A206" s="1" t="s">
         <v>143</v>
       </c>
@@ -11227,7 +11231,7 @@
         <v>6.85</v>
       </c>
     </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A207" s="1" t="s">
         <v>144</v>
       </c>
@@ -11274,7 +11278,7 @@
         <v>8.06</v>
       </c>
     </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A208" s="1" t="s">
         <v>145</v>
       </c>
@@ -11321,7 +11325,7 @@
         <v>5.89</v>
       </c>
     </row>
-    <row r="209" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A209" s="1" t="s">
         <v>146</v>
       </c>
@@ -11368,7 +11372,7 @@
         <v>7.07</v>
       </c>
     </row>
-    <row r="210" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A210" s="1" t="s">
         <v>147</v>
       </c>
@@ -11415,7 +11419,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="211" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A211" s="1" t="s">
         <v>148</v>
       </c>
@@ -11462,7 +11466,7 @@
         <v>2.66</v>
       </c>
     </row>
-    <row r="212" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A212" s="1" t="s">
         <v>149</v>
       </c>
@@ -11509,7 +11513,7 @@
         <v>2.2200000000000002</v>
       </c>
     </row>
-    <row r="213" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A213" s="1" t="s">
         <v>150</v>
       </c>
@@ -11556,7 +11560,7 @@
         <v>5.31</v>
       </c>
     </row>
-    <row r="214" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A214" s="1" t="s">
         <v>151</v>
       </c>
@@ -11603,7 +11607,7 @@
         <v>4.91</v>
       </c>
     </row>
-    <row r="215" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A215" s="1" t="s">
         <v>152</v>
       </c>
@@ -11650,7 +11654,7 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="216" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A216" s="1" t="s">
         <v>153</v>
       </c>
@@ -11697,7 +11701,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A217" s="1" t="s">
         <v>154</v>
       </c>
@@ -11744,7 +11748,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="218" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A218" s="1" t="s">
         <v>155</v>
       </c>
@@ -11791,7 +11795,7 @@
         <v>8.32</v>
       </c>
     </row>
-    <row r="219" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A219" s="1" t="s">
         <v>156</v>
       </c>
@@ -11838,7 +11842,7 @@
         <v>7.91</v>
       </c>
     </row>
-    <row r="220" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A220" s="1" t="s">
         <v>157</v>
       </c>
@@ -11885,7 +11889,7 @@
         <v>8.34</v>
       </c>
     </row>
-    <row r="221" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A221" s="1" t="s">
         <v>158</v>
       </c>
@@ -11932,7 +11936,7 @@
         <v>3.62</v>
       </c>
     </row>
-    <row r="222" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A222" s="1" t="s">
         <v>159</v>
       </c>
@@ -11979,7 +11983,7 @@
         <v>6.57</v>
       </c>
     </row>
-    <row r="223" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A223" s="1" t="s">
         <v>160</v>
       </c>
@@ -12026,7 +12030,7 @@
         <v>8.86</v>
       </c>
     </row>
-    <row r="224" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="s">
         <v>161</v>
       </c>
@@ -12073,7 +12077,7 @@
         <v>8.9499999999999993</v>
       </c>
     </row>
-    <row r="225" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A225" s="1" t="s">
         <v>162</v>
       </c>
@@ -12120,7 +12124,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="226" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A226" s="1" t="s">
         <v>163</v>
       </c>
@@ -12167,7 +12171,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="227" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A227" s="1" t="s">
         <v>164</v>
       </c>
@@ -12214,7 +12218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="s">
         <v>165</v>
       </c>
@@ -12261,7 +12265,7 @@
         <v>1.43</v>
       </c>
     </row>
-    <row r="229" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A229" s="1" t="s">
         <v>166</v>
       </c>
@@ -12308,7 +12312,7 @@
         <v>2.2400000000000002</v>
       </c>
     </row>
-    <row r="230" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A230" s="1" t="s">
         <v>167</v>
       </c>
@@ -12355,7 +12359,7 @@
         <v>2.4700000000000002</v>
       </c>
     </row>
-    <row r="231" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A231" s="1" t="s">
         <v>168</v>
       </c>
@@ -12402,7 +12406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="232" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A232" s="1" t="s">
         <v>169</v>
       </c>
@@ -12449,7 +12453,7 @@
         <v>2.73</v>
       </c>
     </row>
-    <row r="233" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A233" s="1" t="s">
         <v>170</v>
       </c>
@@ -12496,7 +12500,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="234" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A234" s="1" t="s">
         <v>171</v>
       </c>
@@ -12543,7 +12547,7 @@
         <v>2.13</v>
       </c>
     </row>
-    <row r="235" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A235" s="1" t="s">
         <v>172</v>
       </c>
@@ -12590,7 +12594,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="236" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A236" s="1" t="s">
         <v>173</v>
       </c>
@@ -12637,7 +12641,7 @@
         <v>5.53</v>
       </c>
     </row>
-    <row r="237" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A237" s="1" t="s">
         <v>174</v>
       </c>
@@ -12684,7 +12688,7 @@
         <v>1.43</v>
       </c>
     </row>
-    <row r="238" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A238" s="1" t="s">
         <v>175</v>
       </c>
@@ -12731,7 +12735,7 @@
         <v>6.65</v>
       </c>
     </row>
-    <row r="239" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A239" s="1" t="s">
         <v>176</v>
       </c>
@@ -12778,7 +12782,7 @@
         <v>4.74</v>
       </c>
     </row>
-    <row r="240" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A240" s="1" t="s">
         <v>177</v>
       </c>
@@ -12825,7 +12829,7 @@
         <v>7.39</v>
       </c>
     </row>
-    <row r="241" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A241" s="1" t="s">
         <v>178</v>
       </c>
@@ -12872,7 +12876,7 @@
         <v>8.5299999999999994</v>
       </c>
     </row>
-    <row r="242" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A242" s="1" t="s">
         <v>179</v>
       </c>
@@ -12919,7 +12923,7 @@
         <v>6.97</v>
       </c>
     </row>
-    <row r="243" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A243" s="1" t="s">
         <v>180</v>
       </c>
@@ -12966,7 +12970,7 @@
         <v>4.67</v>
       </c>
     </row>
-    <row r="244" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A244" s="1" t="s">
         <v>181</v>
       </c>
@@ -13013,7 +13017,7 @@
         <v>6.44</v>
       </c>
     </row>
-    <row r="245" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A245" s="1" t="s">
         <v>182</v>
       </c>
@@ -13060,7 +13064,7 @@
         <v>6.21</v>
       </c>
     </row>
-    <row r="246" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A246" s="1" t="s">
         <v>183</v>
       </c>
@@ -13107,7 +13111,7 @@
         <v>5.85</v>
       </c>
     </row>
-    <row r="247" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A247" s="1" t="s">
         <v>184</v>
       </c>
@@ -13154,7 +13158,7 @@
         <v>10.93</v>
       </c>
     </row>
-    <row r="248" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A248" s="1" t="s">
         <v>185</v>
       </c>
@@ -13201,7 +13205,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="249" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A249" s="1" t="s">
         <v>186</v>
       </c>
@@ -13248,7 +13252,7 @@
         <v>6.09</v>
       </c>
     </row>
-    <row r="250" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A250" s="1" t="s">
         <v>187</v>
       </c>
@@ -13295,7 +13299,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="251" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A251" s="1" t="s">
         <v>188</v>
       </c>
@@ -13342,7 +13346,7 @@
         <v>2.68</v>
       </c>
     </row>
-    <row r="252" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A252" s="1" t="s">
         <v>189</v>
       </c>
@@ -13389,7 +13393,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="253" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A253" s="1" t="s">
         <v>190</v>
       </c>
@@ -13436,7 +13440,7 @@
         <v>1.74</v>
       </c>
     </row>
-    <row r="254" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A254" s="1" t="s">
         <v>191</v>
       </c>
@@ -13483,7 +13487,7 @@
         <v>7.67</v>
       </c>
     </row>
-    <row r="255" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A255" s="1" t="s">
         <v>192</v>
       </c>
@@ -13530,7 +13534,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="256" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A256" s="1" t="s">
         <v>193</v>
       </c>
@@ -13577,7 +13581,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="257" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A257" s="1" t="s">
         <v>194</v>
       </c>
@@ -13624,7 +13628,7 @@
         <v>1.46</v>
       </c>
     </row>
-    <row r="258" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A258" s="1" t="s">
         <v>195</v>
       </c>
@@ -13671,7 +13675,7 @@
         <v>5.79</v>
       </c>
     </row>
-    <row r="259" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A259" s="1" t="s">
         <v>196</v>
       </c>
@@ -13718,7 +13722,7 @@
         <v>8.19</v>
       </c>
     </row>
-    <row r="260" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A260" s="1" t="s">
         <v>197</v>
       </c>
@@ -13765,7 +13769,7 @@
         <v>11.75</v>
       </c>
     </row>
-    <row r="261" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A261" s="1" t="s">
         <v>198</v>
       </c>
@@ -13812,7 +13816,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="262" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A262" s="1" t="s">
         <v>199</v>
       </c>
@@ -13859,7 +13863,7 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="263" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A263" s="1" t="s">
         <v>200</v>
       </c>
@@ -13906,7 +13910,7 @@
         <v>2.81</v>
       </c>
     </row>
-    <row r="264" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A264" s="1" t="s">
         <v>201</v>
       </c>
@@ -13953,7 +13957,7 @@
         <v>7.05</v>
       </c>
     </row>
-    <row r="265" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A265" s="1" t="s">
         <v>202</v>
       </c>
@@ -14000,7 +14004,7 @@
         <v>6.75</v>
       </c>
     </row>
-    <row r="266" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A266" s="1" t="s">
         <v>203</v>
       </c>
@@ -14047,7 +14051,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="267" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A267" s="1" t="s">
         <v>204</v>
       </c>
@@ -14094,7 +14098,7 @@
         <v>6.14</v>
       </c>
     </row>
-    <row r="268" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A268" s="1" t="s">
         <v>205</v>
       </c>
@@ -14141,7 +14145,7 @@
         <v>4.78</v>
       </c>
     </row>
-    <row r="269" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A269" s="1" t="s">
         <v>206</v>
       </c>
@@ -14188,7 +14192,7 @@
         <v>2.54</v>
       </c>
     </row>
-    <row r="270" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A270" s="1" t="s">
         <v>207</v>
       </c>
@@ -14235,7 +14239,7 @@
         <v>14.55</v>
       </c>
     </row>
-    <row r="271" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A271" s="1" t="s">
         <v>208</v>
       </c>
@@ -14282,7 +14286,7 @@
         <v>14.35</v>
       </c>
     </row>
-    <row r="272" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A272" s="1" t="s">
         <v>209</v>
       </c>
@@ -14329,7 +14333,7 @@
         <v>14.22</v>
       </c>
     </row>
-    <row r="273" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A273" s="1" t="s">
         <v>210</v>
       </c>
@@ -14376,7 +14380,7 @@
         <v>2.74</v>
       </c>
     </row>
-    <row r="274" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A274" s="1" t="s">
         <v>211</v>
       </c>
@@ -14423,7 +14427,7 @@
         <v>5.89</v>
       </c>
     </row>
-    <row r="275" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A275" s="1" t="s">
         <v>212</v>
       </c>
@@ -14470,7 +14474,7 @@
         <v>8.2100000000000009</v>
       </c>
     </row>
-    <row r="276" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A276" s="1" t="s">
         <v>213</v>
       </c>
@@ -14517,7 +14521,7 @@
         <v>6.73</v>
       </c>
     </row>
-    <row r="277" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A277" s="1" t="s">
         <v>214</v>
       </c>
@@ -14564,7 +14568,7 @@
         <v>11.79</v>
       </c>
     </row>
-    <row r="278" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A278" s="1" t="s">
         <v>215</v>
       </c>
@@ -14611,7 +14615,7 @@
         <v>16.05</v>
       </c>
     </row>
-    <row r="279" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A279" s="1" t="s">
         <v>216</v>
       </c>
@@ -14658,7 +14662,7 @@
         <v>14.85</v>
       </c>
     </row>
-    <row r="280" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A280" s="1" t="s">
         <v>217</v>
       </c>
@@ -14705,7 +14709,7 @@
         <v>13.07</v>
       </c>
     </row>
-    <row r="281" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A281" s="1" t="s">
         <v>218</v>
       </c>
@@ -14752,7 +14756,7 @@
         <v>7.59</v>
       </c>
     </row>
-    <row r="282" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A282" s="1" t="s">
         <v>219</v>
       </c>
@@ -14799,7 +14803,7 @@
         <v>8.26</v>
       </c>
     </row>
-    <row r="283" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A283" s="1" t="s">
         <v>220</v>
       </c>
@@ -14846,7 +14850,7 @@
         <v>5.39</v>
       </c>
     </row>
-    <row r="284" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A284" s="1" t="s">
         <v>221</v>
       </c>
@@ -14893,7 +14897,7 @@
         <v>11.78</v>
       </c>
     </row>
-    <row r="285" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A285" s="1" t="s">
         <v>222</v>
       </c>
@@ -14940,7 +14944,7 @@
         <v>15.81</v>
       </c>
     </row>
-    <row r="286" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A286" s="1" t="s">
         <v>223</v>
       </c>
@@ -14987,7 +14991,7 @@
         <v>4.16</v>
       </c>
     </row>
-    <row r="287" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A287" s="1" t="s">
         <v>224</v>
       </c>
@@ -15034,7 +15038,7 @@
         <v>3.67</v>
       </c>
     </row>
-    <row r="288" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A288" s="1" t="s">
         <v>225</v>
       </c>
@@ -15081,7 +15085,7 @@
         <v>3.61</v>
       </c>
     </row>
-    <row r="289" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A289" s="1" t="s">
         <v>226</v>
       </c>
@@ -15128,7 +15132,7 @@
         <v>17.13</v>
       </c>
     </row>
-    <row r="290" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A290" s="1" t="s">
         <v>227</v>
       </c>
@@ -15175,7 +15179,7 @@
         <v>17.59</v>
       </c>
     </row>
-    <row r="291" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A291" s="1" t="s">
         <v>228</v>
       </c>
@@ -15222,7 +15226,7 @@
         <v>12.44</v>
       </c>
     </row>
-    <row r="292" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A292" s="1" t="s">
         <v>229</v>
       </c>
@@ -15269,7 +15273,7 @@
         <v>18.28</v>
       </c>
     </row>
-    <row r="293" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A293" s="1" t="s">
         <v>230</v>
       </c>
@@ -15316,7 +15320,7 @@
         <v>6.53</v>
       </c>
     </row>
-    <row r="294" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A294" s="1" t="s">
         <v>231</v>
       </c>
@@ -15363,7 +15367,7 @@
         <v>7.94</v>
       </c>
     </row>
-    <row r="295" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A295" s="1" t="s">
         <v>232</v>
       </c>
@@ -15410,7 +15414,7 @@
         <v>17.510000000000002</v>
       </c>
     </row>
-    <row r="296" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A296" s="1" t="s">
         <v>233</v>
       </c>
@@ -15457,7 +15461,7 @@
         <v>18.79</v>
       </c>
     </row>
-    <row r="297" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A297" s="1" t="s">
         <v>234</v>
       </c>
@@ -15504,7 +15508,7 @@
         <v>10.32</v>
       </c>
     </row>
-    <row r="298" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A298" s="1" t="s">
         <v>235</v>
       </c>
@@ -15551,7 +15555,7 @@
         <v>9.52</v>
       </c>
     </row>
-    <row r="299" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A299" s="1" t="s">
         <v>236</v>
       </c>
@@ -15598,7 +15602,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="300" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A300" s="1" t="s">
         <v>237</v>
       </c>
@@ -15645,7 +15649,7 @@
         <v>18.43</v>
       </c>
     </row>
-    <row r="301" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A301" s="1" t="s">
         <v>238</v>
       </c>
@@ -15692,7 +15696,7 @@
         <v>17.61</v>
       </c>
     </row>
-    <row r="302" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A302" s="1" t="s">
         <v>239</v>
       </c>
@@ -15739,7 +15743,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="303" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A303" s="1" t="s">
         <v>240</v>
       </c>
@@ -15786,7 +15790,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="304" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A304" s="1" t="s">
         <v>241</v>
       </c>
@@ -15833,7 +15837,7 @@
         <v>4.04</v>
       </c>
     </row>
-    <row r="305" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A305" s="1" t="s">
         <v>242</v>
       </c>
@@ -15880,7 +15884,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="306" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A306" s="1" t="s">
         <v>243</v>
       </c>
@@ -15927,7 +15931,7 @@
         <v>18.489999999999998</v>
       </c>
     </row>
-    <row r="307" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A307" s="1" t="s">
         <v>244</v>
       </c>
@@ -15974,7 +15978,7 @@
         <v>17.7</v>
       </c>
     </row>
-    <row r="308" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A308" s="1" t="s">
         <v>245</v>
       </c>
@@ -16021,7 +16025,7 @@
         <v>11.55</v>
       </c>
     </row>
-    <row r="309" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A309" s="1" t="s">
         <v>246</v>
       </c>
@@ -16068,7 +16072,7 @@
         <v>2.34</v>
       </c>
     </row>
-    <row r="310" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A310" s="1" t="s">
         <v>247</v>
       </c>
@@ -16115,7 +16119,7 @@
         <v>4.8099999999999996</v>
       </c>
     </row>
-    <row r="311" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A311" s="1" t="s">
         <v>248</v>
       </c>
@@ -16162,7 +16166,7 @@
         <v>19.39</v>
       </c>
     </row>
-    <row r="312" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A312" s="1" t="s">
         <v>249</v>
       </c>
@@ -16209,7 +16213,7 @@
         <v>16.12</v>
       </c>
     </row>
-    <row r="313" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A313" s="1" t="s">
         <v>250</v>
       </c>
@@ -16256,7 +16260,7 @@
         <v>19.22</v>
       </c>
     </row>
-    <row r="314" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A314" s="1" t="s">
         <v>251</v>
       </c>
@@ -16303,7 +16307,7 @@
         <v>20.6</v>
       </c>
     </row>
-    <row r="315" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A315" s="1" t="s">
         <v>252</v>
       </c>
@@ -16350,7 +16354,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="316" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A316" s="1" t="s">
         <v>253</v>
       </c>
@@ -16397,7 +16401,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="317" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A317" s="1" t="s">
         <v>254</v>
       </c>
@@ -16444,7 +16448,7 @@
         <v>21.37</v>
       </c>
     </row>
-    <row r="318" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A318" s="1" t="s">
         <v>255</v>
       </c>
@@ -16491,7 +16495,7 @@
         <v>15.05</v>
       </c>
     </row>
-    <row r="319" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A319" s="1" t="s">
         <v>256</v>
       </c>
@@ -16538,7 +16542,7 @@
         <v>17.190000000000001</v>
       </c>
     </row>
-    <row r="320" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A320" s="1" t="s">
         <v>257</v>
       </c>
@@ -16585,7 +16589,7 @@
         <v>20.89</v>
       </c>
     </row>
-    <row r="321" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A321" s="1" t="s">
         <v>258</v>
       </c>
@@ -16632,7 +16636,7 @@
         <v>20.58</v>
       </c>
     </row>
-    <row r="322" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A322" s="1" t="s">
         <v>259</v>
       </c>
@@ -16679,7 +16683,7 @@
         <v>15.71</v>
       </c>
     </row>
-    <row r="323" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A323" s="1" t="s">
         <v>260</v>
       </c>
@@ -16726,7 +16730,7 @@
         <v>6.02</v>
       </c>
     </row>
-    <row r="324" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A324" s="1" t="s">
         <v>261</v>
       </c>
@@ -16773,7 +16777,7 @@
         <v>19.77</v>
       </c>
     </row>
-    <row r="325" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A325" s="1" t="s">
         <v>262</v>
       </c>
@@ -16820,7 +16824,7 @@
         <v>22.48</v>
       </c>
     </row>
-    <row r="326" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A326" s="1" t="s">
         <v>263</v>
       </c>
@@ -16867,7 +16871,7 @@
         <v>21.3</v>
       </c>
     </row>
-    <row r="327" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A327" s="1" t="s">
         <v>264</v>
       </c>
@@ -16914,7 +16918,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="328" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A328" s="1" t="s">
         <v>265</v>
       </c>
@@ -16961,7 +16965,7 @@
         <v>6.07</v>
       </c>
     </row>
-    <row r="329" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A329" s="1" t="s">
         <v>266</v>
       </c>
@@ -17008,7 +17012,7 @@
         <v>6.56</v>
       </c>
     </row>
-    <row r="330" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A330" s="1" t="s">
         <v>267</v>
       </c>
@@ -17055,7 +17059,7 @@
         <v>11.95</v>
       </c>
     </row>
-    <row r="331" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A331" s="1" t="s">
         <v>268</v>
       </c>
@@ -17102,7 +17106,7 @@
         <v>23.28</v>
       </c>
     </row>
-    <row r="332" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A332" s="1" t="s">
         <v>269</v>
       </c>
@@ -17149,7 +17153,7 @@
         <v>17.239999999999998</v>
       </c>
     </row>
-    <row r="333" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A333" s="1" t="s">
         <v>270</v>
       </c>
@@ -17196,7 +17200,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="334" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A334" s="1" t="s">
         <v>271</v>
       </c>
@@ -17243,7 +17247,7 @@
         <v>10.24</v>
       </c>
     </row>
-    <row r="335" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A335" s="1" t="s">
         <v>272</v>
       </c>
@@ -17290,7 +17294,7 @@
         <v>4.45</v>
       </c>
     </row>
-    <row r="336" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A336" s="1" t="s">
         <v>273</v>
       </c>
@@ -17337,7 +17341,7 @@
         <v>11.66</v>
       </c>
     </row>
-    <row r="337" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A337" s="1" t="s">
         <v>274</v>
       </c>
@@ -17384,7 +17388,7 @@
         <v>6.35</v>
       </c>
     </row>
-    <row r="338" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A338" s="1" t="s">
         <v>275</v>
       </c>
@@ -17431,7 +17435,7 @@
         <v>6.02</v>
       </c>
     </row>
-    <row r="339" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A339" s="1" t="s">
         <v>276</v>
       </c>
@@ -17478,7 +17482,7 @@
         <v>21.65</v>
       </c>
     </row>
-    <row r="340" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A340" s="1" t="s">
         <v>277</v>
       </c>
@@ -17525,7 +17529,7 @@
         <v>22.41</v>
       </c>
     </row>
-    <row r="341" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A341" s="1" t="s">
         <v>278</v>
       </c>
@@ -17572,7 +17576,7 @@
         <v>17.59</v>
       </c>
     </row>
-    <row r="342" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A342" s="1" t="s">
         <v>279</v>
       </c>
@@ -17619,7 +17623,7 @@
         <v>12.35</v>
       </c>
     </row>
-    <row r="343" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A343" s="1" t="s">
         <v>280</v>
       </c>
@@ -17666,7 +17670,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="344" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A344" s="1" t="s">
         <v>281</v>
       </c>
@@ -17713,7 +17717,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="345" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A345" s="1" t="s">
         <v>282</v>
       </c>
@@ -17760,7 +17764,7 @@
         <v>19.63</v>
       </c>
     </row>
-    <row r="346" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A346" s="1" t="s">
         <v>283</v>
       </c>
@@ -17807,7 +17811,7 @@
         <v>7.87</v>
       </c>
     </row>
-    <row r="347" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A347" s="1" t="s">
         <v>284</v>
       </c>
@@ -17854,7 +17858,7 @@
         <v>11.16</v>
       </c>
     </row>
-    <row r="348" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A348" s="1" t="s">
         <v>285</v>
       </c>
@@ -17901,7 +17905,7 @@
         <v>24.88</v>
       </c>
     </row>
-    <row r="349" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A349" s="1" t="s">
         <v>286</v>
       </c>
@@ -17948,7 +17952,7 @@
         <v>22.12</v>
       </c>
     </row>
-    <row r="350" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A350" s="1" t="s">
         <v>287</v>
       </c>
@@ -17995,7 +17999,7 @@
         <v>24.53</v>
       </c>
     </row>
-    <row r="351" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A351" s="1" t="s">
         <v>288</v>
       </c>
@@ -18042,7 +18046,7 @@
         <v>24.53</v>
       </c>
     </row>
-    <row r="352" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A352" s="1" t="s">
         <v>289</v>
       </c>
@@ -18089,7 +18093,7 @@
         <v>23.59</v>
       </c>
     </row>
-    <row r="353" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A353" s="1" t="s">
         <v>290</v>
       </c>
@@ -18136,7 +18140,7 @@
         <v>9.4499999999999993</v>
       </c>
     </row>
-    <row r="354" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A354" s="1" t="s">
         <v>291</v>
       </c>
@@ -18183,7 +18187,7 @@
         <v>15.03</v>
       </c>
     </row>
-    <row r="355" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A355" s="1" t="s">
         <v>292</v>
       </c>
@@ -18230,7 +18234,7 @@
         <v>17.39</v>
       </c>
     </row>
-    <row r="356" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A356" s="1" t="s">
         <v>293</v>
       </c>
@@ -18277,7 +18281,7 @@
         <v>4.88</v>
       </c>
     </row>
-    <row r="357" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A357" s="1" t="s">
         <v>294</v>
       </c>
@@ -18324,7 +18328,7 @@
         <v>21.56</v>
       </c>
     </row>
-    <row r="358" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A358" s="1" t="s">
         <v>295</v>
       </c>
@@ -18371,7 +18375,7 @@
         <v>18.54</v>
       </c>
     </row>
-    <row r="359" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A359" s="1" t="s">
         <v>296</v>
       </c>
@@ -18418,7 +18422,7 @@
         <v>19.96</v>
       </c>
     </row>
-    <row r="360" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A360" s="1" t="s">
         <v>297</v>
       </c>
@@ -18465,7 +18469,7 @@
         <v>21.85</v>
       </c>
     </row>
-    <row r="361" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A361" s="1" t="s">
         <v>298</v>
       </c>
@@ -18512,7 +18516,7 @@
         <v>17.73</v>
       </c>
     </row>
-    <row r="362" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A362" s="1" t="s">
         <v>299</v>
       </c>
@@ -18559,7 +18563,7 @@
         <v>14.33</v>
       </c>
     </row>
-    <row r="363" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A363" s="1" t="s">
         <v>300</v>
       </c>
@@ -18606,7 +18610,7 @@
         <v>17.66</v>
       </c>
     </row>
-    <row r="364" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A364" s="1" t="s">
         <v>301</v>
       </c>
@@ -18653,7 +18657,7 @@
         <v>14.41</v>
       </c>
     </row>
-    <row r="365" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A365" s="1" t="s">
         <v>302</v>
       </c>
@@ -18700,7 +18704,7 @@
         <v>17.510000000000002</v>
       </c>
     </row>
-    <row r="366" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A366" s="1" t="s">
         <v>303</v>
       </c>

</xml_diff>